<commit_message>
add comment to Data_Only
</commit_message>
<xml_diff>
--- a/202304 Табель ОГМ ПК 250.xlsx
+++ b/202304 Табель ОГМ ПК 250.xlsx
@@ -5148,17 +5148,29 @@
     <mergeCell ref="AL44:AP44"/>
     <mergeCell ref="AJ8:AU8"/>
   </mergeCells>
-  <dataValidations count="6">
-    <dataValidation sqref="E13:AI35" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+  <dataValidations count="10">
+    <dataValidation sqref="E13:AI35" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'Main'!$E$48:$AB$48</formula1>
     </dataValidation>
-    <dataValidation sqref="E45:AI45" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E45:AI45" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'Main'!$AF$48:$AI$48</formula1>
     </dataValidation>
-    <dataValidation sqref="E13:AI35" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E13:AI35" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'Main'!$E$48:$AB$48</formula1>
     </dataValidation>
-    <dataValidation sqref="E45:AI45" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="E45:AI45" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>'Main'!$AF$48:$AI$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E13:AI35" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E45:AI45" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>'Main'!$AF$48:$AI$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E13:AI35" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E45:AI45" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>'Main'!$AF$48:$AI$48</formula1>
     </dataValidation>
     <dataValidation sqref="E13:AI35" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">

</xml_diff>